<commit_message>
update - import mailer from Excel file
</commit_message>
<xml_diff>
--- a/MNPOST/Templates/mailer.template.xlsx
+++ b/MNPOST/Templates/mailer.template.xlsx
@@ -87,7 +87,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,33 +103,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -181,12 +185,12 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -471,90 +475,90 @@
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B14" sqref="B14"/>
+      <pane xSplit="2" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="44.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="28" style="3" customWidth="1"/>
-    <col min="6" max="6" width="26.42578125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="27.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="24" style="3" customWidth="1"/>
-    <col min="9" max="9" width="29.42578125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="23.85546875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="23.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="21.5703125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="13.140625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" style="2" customWidth="1"/>
-    <col min="17" max="17" width="26.7109375" style="2" customWidth="1"/>
-    <col min="18" max="18" width="26.28515625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="18.7109375" style="2" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="23.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="44.85546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="28" style="6" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="24" style="6" customWidth="1"/>
+    <col min="9" max="9" width="34.42578125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="23.85546875" style="6" customWidth="1"/>
+    <col min="12" max="12" width="23.140625" style="6" customWidth="1"/>
+    <col min="13" max="13" width="21.5703125" style="5" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" style="5" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="5" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" style="5" customWidth="1"/>
+    <col min="17" max="17" width="26.7109375" style="5" customWidth="1"/>
+    <col min="18" max="18" width="26.28515625" style="5" customWidth="1"/>
+    <col min="19" max="19" width="18.7109375" style="5" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>